<commit_message>
Upload excel To Admin Pannel
</commit_message>
<xml_diff>
--- a/Dashboard/media/test_excel.xlsx
+++ b/Dashboard/media/test_excel.xlsx
@@ -8,17 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\__gitam__\DashBoard-BackEnd\Dashboard\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2767C2B-9082-4B48-90D9-CAA75CC5BD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6AA0CD-432E-4EEA-AC77-849E9F403D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8040" yWindow="270" windowWidth="21600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -406,12 +413,12 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="1" max="1" width="106.140625" customWidth="1"/>
     <col min="2" max="2" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>